<commit_message>
Converted AboveGround to Aboveground harvestable in Ryegrass.apsimx
</commit_message>
<xml_diff>
--- a/Prototypes/Ryegrass/KairiObserved9194.xlsx
+++ b/Prototypes/Ryegrass/KairiObserved9194.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jessica\GIT\ApsimX\ApsimX\Tests\Validation\Ryegrass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jessica\GIT\ApsimX\ApsimX\Prototypes\Ryegrass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703EC0EB-E8C6-4654-BA89-B4AB9BA96AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CF0DA4-7E42-481D-912D-1A3905CD7545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="81480" yWindow="15" windowWidth="38640" windowHeight="21120" xr2:uid="{C895F722-8CE5-4DBC-9625-32A2544C10FD}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15943" xr2:uid="{C895F722-8CE5-4DBC-9625-32A2544C10FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$A$343</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$A$341</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="26">
   <si>
     <t>SimulationName</t>
   </si>
@@ -511,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88836581-3558-4849-859A-2A7B0780DAF8}">
-  <dimension ref="A1:E250"/>
+  <dimension ref="A1:E248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="O250" sqref="O249:O250"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="D249" sqref="D249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3438,10 +3438,10 @@
         <v>24</v>
       </c>
       <c r="B234" s="3">
-        <v>34213</v>
+        <v>34608</v>
       </c>
       <c r="C234" s="1">
-        <v>4.9410999999999997E-2</v>
+        <v>4.9540000000000001E-2</v>
       </c>
       <c r="E234" s="1">
         <v>100</v>
@@ -3452,10 +3452,10 @@
         <v>24</v>
       </c>
       <c r="B235" s="3">
-        <v>34608</v>
+        <v>34639</v>
       </c>
       <c r="C235" s="1">
-        <v>4.9540000000000001E-2</v>
+        <v>5.5147000000000002E-2</v>
       </c>
       <c r="E235" s="1">
         <v>100</v>
@@ -3466,10 +3466,10 @@
         <v>24</v>
       </c>
       <c r="B236" s="3">
-        <v>34639</v>
+        <v>34669</v>
       </c>
       <c r="C236" s="1">
-        <v>5.5147000000000002E-2</v>
+        <v>4.3840999999999998E-2</v>
       </c>
       <c r="E236" s="1">
         <v>100</v>
@@ -3477,16 +3477,13 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A237" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B237" s="3">
-        <v>34669</v>
-      </c>
-      <c r="C237" s="1">
-        <v>4.3840999999999998E-2</v>
+        <v>34335</v>
       </c>
       <c r="E237" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.4">
@@ -3494,7 +3491,7 @@
         <v>25</v>
       </c>
       <c r="B238" s="3">
-        <v>34335</v>
+        <v>34366</v>
       </c>
       <c r="E238" s="1">
         <v>150</v>
@@ -3505,7 +3502,7 @@
         <v>25</v>
       </c>
       <c r="B239" s="3">
-        <v>34366</v>
+        <v>34394</v>
       </c>
       <c r="E239" s="1">
         <v>150</v>
@@ -3516,7 +3513,7 @@
         <v>25</v>
       </c>
       <c r="B240" s="3">
-        <v>34394</v>
+        <v>34425</v>
       </c>
       <c r="E240" s="1">
         <v>150</v>
@@ -3527,7 +3524,7 @@
         <v>25</v>
       </c>
       <c r="B241" s="3">
-        <v>34425</v>
+        <v>34455</v>
       </c>
       <c r="E241" s="1">
         <v>150</v>
@@ -3538,7 +3535,10 @@
         <v>25</v>
       </c>
       <c r="B242" s="3">
-        <v>34455</v>
+        <v>34486</v>
+      </c>
+      <c r="C242" s="1">
+        <v>5.3810000000000004E-2</v>
       </c>
       <c r="E242" s="1">
         <v>150</v>
@@ -3549,10 +3549,10 @@
         <v>25</v>
       </c>
       <c r="B243" s="3">
-        <v>34486</v>
+        <v>34516</v>
       </c>
       <c r="C243" s="1">
-        <v>5.3810000000000004E-2</v>
+        <v>5.3352000000000004E-2</v>
       </c>
       <c r="E243" s="1">
         <v>150</v>
@@ -3563,10 +3563,10 @@
         <v>25</v>
       </c>
       <c r="B244" s="3">
-        <v>34516</v>
+        <v>34547</v>
       </c>
       <c r="C244" s="1">
-        <v>5.3352000000000004E-2</v>
+        <v>5.8665000000000002E-2</v>
       </c>
       <c r="E244" s="1">
         <v>150</v>
@@ -3577,10 +3577,7 @@
         <v>25</v>
       </c>
       <c r="B245" s="3">
-        <v>34547</v>
-      </c>
-      <c r="C245" s="1">
-        <v>5.8665000000000002E-2</v>
+        <v>34608</v>
       </c>
       <c r="E245" s="1">
         <v>150</v>
@@ -3591,10 +3588,7 @@
         <v>25</v>
       </c>
       <c r="B246" s="3">
-        <v>34213</v>
-      </c>
-      <c r="C246" s="1">
-        <v>4.4721999999999998E-2</v>
+        <v>34639</v>
       </c>
       <c r="E246" s="1">
         <v>150</v>
@@ -3605,7 +3599,10 @@
         <v>25</v>
       </c>
       <c r="B247" s="3">
-        <v>34608</v>
+        <v>34669</v>
+      </c>
+      <c r="C247" s="1">
+        <v>4.1399999999999999E-2</v>
       </c>
       <c r="E247" s="1">
         <v>150</v>
@@ -3616,39 +3613,14 @@
         <v>25</v>
       </c>
       <c r="B248" s="3">
-        <v>34639</v>
-      </c>
-      <c r="E248" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A249" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B249" s="3">
-        <v>34669</v>
-      </c>
-      <c r="C249" s="1">
-        <v>4.1399999999999999E-2</v>
-      </c>
-      <c r="E249" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A250" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B250" s="3">
         <v>34699</v>
       </c>
-      <c r="D250" s="1">
+      <c r="D248" s="1">
         <v>996.78000000000009</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A343" xr:uid="{88836581-3558-4849-859A-2A7B0780DAF8}"/>
+  <autoFilter ref="A1:A341" xr:uid="{88836581-3558-4849-859A-2A7B0780DAF8}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>